<commit_message>
updating AUTH in xlsx
</commit_message>
<xml_diff>
--- a/Windows_DS.xlsx
+++ b/Windows_DS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051EAE2D-5E03-4B0C-969A-C279F7C8B4E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB9C6DF-E971-4FAC-A1C4-3B2AEEFAB350}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Marius</t>
+  </si>
+  <si>
+    <t>AUTH</t>
   </si>
 </sst>
 </file>
@@ -538,7 +541,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +584,7 @@
     </row>
     <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
fixed dependencies in xlsx
</commit_message>
<xml_diff>
--- a/Windows_DS.xlsx
+++ b/Windows_DS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB9C6DF-E971-4FAC-A1C4-3B2AEEFAB350}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5107F5C3-2C0F-4EEC-8CCD-522D8E9F497F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Powershell(y/n)</t>
-  </si>
-  <si>
-    <t>Authentication</t>
   </si>
   <si>
     <t>the purpose of...</t>
@@ -584,95 +581,95 @@
     </row>
     <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
         <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -680,16 +677,16 @@
     </row>
     <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -697,14 +694,14 @@
     </row>
     <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -712,28 +709,28 @@
     </row>
     <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -741,14 +738,14 @@
     </row>
     <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>